<commit_message>
Some of my updated data files as i was reprocessing the data with the updated incidence data
</commit_message>
<xml_diff>
--- a/02_Cleaned_Data/CleanedDataDictinary.xlsx
+++ b/02_Cleaned_Data/CleanedDataDictinary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac King\OneDrive\Documents\LSHTM_23\Thesis\Lima_Dengue\02_Cleaned_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20863A2E-BE22-429E-AFB1-093F383B3525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A897856-1AD8-48B8-9966-64494E58A085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{71660202-5B80-45C1-9BB3-D434AA68B6D5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Data Dictionary for Cleaned Data</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>(Num)</t>
+  </si>
+  <si>
+    <t>Grave Dengue</t>
   </si>
 </sst>
 </file>
@@ -121,13 +124,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85507F7-0458-494A-86A9-0B12786824E9}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,13 +477,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -491,10 +494,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -542,6 +545,14 @@
       </c>
       <c r="B9" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>